<commit_message>
LAND ARCH UG MODULES
</commit_message>
<xml_diff>
--- a/Datasets/UCD_EngArch_Path_LandArch_UG_Modules.xlsx
+++ b/Datasets/UCD_EngArch_Path_LandArch_UG_Modules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\SATLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alanh\Documents\GitHub\ChatGPTAssessment\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F749499-5620-4A73-A18C-9C2A4EBA2690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C0C3FB-2D00-4844-96DE-D9C1702C227E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C7146B4A-4439-46E0-B60E-DB05B9DBCCC1}"/>
   </bookViews>
@@ -543,7 +543,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G2:G30"/>
+      <selection activeCell="H30" sqref="A1:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>